<commit_message>
fix: :card_file_box: FIX DATA 2015
</commit_message>
<xml_diff>
--- a/apps/load_data/2015/01/PLMOVMAE.xlsx
+++ b/apps/load_data/2015/01/PLMOVMAE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NOMBRADOS -2015\HHY0115\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HHY ACTUALIZADOS\2015\HHY0115\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A75797-8A83-427D-9D5D-C0A903730029}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D2AB77-A8CD-4A2B-9CC1-6266A0B8935C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="10305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="PLMOVMAE" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PLMOVMAE!$A$1:$CF$258</definedName>
     <definedName name="_xlnm.Database">PLMOVMAE!$A$1:$CF$253</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -8384,8 +8385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CF258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A240" workbookViewId="0">
-      <selection activeCell="O263" sqref="O263"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52708,6 +52709,7 @@
       <c r="CF258" s="4"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:CF258" xr:uid="{D8DCAFA4-ECC3-4647-B65E-672A2F84D795}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>